<commit_message>
Putting art asset list
</commit_message>
<xml_diff>
--- a/Documentation/Asset Lists.xlsx
+++ b/Documentation/Asset Lists.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sound List" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Tech Lead Asset List:</t>
   </si>
@@ -74,6 +74,75 @@
   </si>
   <si>
     <t xml:space="preserve">Wind  </t>
+  </si>
+  <si>
+    <t>Trex idle</t>
+  </si>
+  <si>
+    <t>Pterodactyl/ animation</t>
+  </si>
+  <si>
+    <t>13 Cactuses</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Reset Button</t>
+  </si>
+  <si>
+    <t>Trex Logo</t>
+  </si>
+  <si>
+    <t>Trex run animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trex death frame </t>
+  </si>
+  <si>
+    <t>Trex crouch/run animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicken run </t>
+  </si>
+  <si>
+    <t>Chicken idle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicken jump </t>
+  </si>
+  <si>
+    <t>chicken coup</t>
+  </si>
+  <si>
+    <t>chicken nest</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seed </t>
+  </si>
+  <si>
+    <t>background</t>
+  </si>
+  <si>
+    <t>ground</t>
+  </si>
+  <si>
+    <t>farmer</t>
+  </si>
+  <si>
+    <t>dog enemy animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sign </t>
+  </si>
+  <si>
+    <t>chicken death</t>
   </si>
 </sst>
 </file>
@@ -422,10 +491,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -435,6 +504,121 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -444,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>